<commit_message>
+ Screen positioning at open is adjusted + code clean up in main_strategy.py + Added new variable for icon + Added icon file + Updated icons_lib.py + Updated api_home.py to show the icon
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
@@ -642,17 +642,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2022-04-13</t>
+          <t>2022-04-21</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY2241318000CE</t>
+          <t>NIFTY2242116850PE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>33</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>29</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -672,39 +672,39 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="V2" t="inlineStr">
         <is>
           <t>NO</t>
@@ -712,202 +712,45 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
+          <t>existing</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>0.6</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
           <t>new</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
         <is>
           <t>YES</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>0.6</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AD2" t="inlineStr">
         <is>
           <t>existing</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
       <c r="AE2" t="inlineStr">
-        <is>
-          <t>Default</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>MARKET</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>MIS</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>NFO</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>NIFTY</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2022-04-13</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>NIFTY2241318000CE</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>0.6</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>existing</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
         <is>
           <t>Default</t>
         </is>

</xml_diff>

<commit_message>
+ upgrade to version to v0.1.8 + update transaction types to variables at required positions + corrected mapping logic for order status.
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
@@ -642,12 +642,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2022-04-21</t>
+          <t>2022-06-09</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY2242116850PE</t>
+          <t>NIFTY2260916500CE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -702,55 +702,212 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>existing</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>0.6</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>existing</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>Default</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>MIS</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2022-06-09</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>NIFTY2260916500CE</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>existing</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>existing</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>0.6</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AD3" t="inlineStr">
         <is>
           <t>new</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>existing</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AE3" t="inlineStr">
         <is>
           <t>Default</t>
         </is>

</xml_diff>

<commit_message>
Fixed sl order transaction type
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -602,7 +602,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -632,22 +632,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>NFO</t>
+          <t>MCX</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>NIFTY</t>
+          <t>CRUDEOIL</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2022-06-09</t>
+          <t>2022-08-19</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY2260916500CE</t>
+          <t>CRUDEOIL22AUGFUT</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -677,27 +677,27 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>Percentage</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0.2</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>Percentage</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>25</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -759,7 +759,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Buy</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -789,22 +789,22 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>NFO</t>
+          <t>MCX</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>NIFTY</t>
+          <t>CRUDEOIL</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2022-06-09</t>
+          <t>2022-08-19</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>NIFTY2260916500CE</t>
+          <t>CRUDEOIL22AUGFUT</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -829,32 +829,32 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>Percentage</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>Percentage</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0.2</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>Percentage</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>25</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">

</xml_diff>